<commit_message>
finish initial feasibility analysis
</commit_message>
<xml_diff>
--- a/data/original_paper_data.xlsx
+++ b/data/original_paper_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\ArClOTs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DAD19D-0EEF-4E0D-ACA1-4988D082D6F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DCC8D5-C366-4EE7-AAF2-2BE7EAEA48DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="815" yWindow="-109" windowWidth="25377" windowHeight="14889" xr2:uid="{2C0A334A-B988-473C-A565-C41D31DD3C5B}"/>
+    <workbookView xWindow="-26192" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{2C0A334A-B988-473C-A565-C41D31DD3C5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add general layout and TOC
</commit_message>
<xml_diff>
--- a/data/original_paper_data.xlsx
+++ b/data/original_paper_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\ArClOTs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40FA191-27DB-4C6C-A2E0-8B61198EEF20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF76891-3FC0-4969-ADA7-CD8CCA2663F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26192" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{2C0A334A-B988-473C-A565-C41D31DD3C5B}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>